<commit_message>
GDE-6675 Keyword and DataSet Updates
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DWE_LIQ/DWELIQ_Functional_TestData.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DWE_LIQ/DWELIQ_Functional_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DWE_LIQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE17451-8D9A-43F0-9009-DBA5EF28D5DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3959DDA-8300-4FBA-94C4-1937B244E723}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FuncVal01" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,12 @@
     <sheet name="FuncVal24" sheetId="21" r:id="rId21"/>
     <sheet name="FuncVal26" sheetId="22" r:id="rId22"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="148">
   <si>
     <t>rowid</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>Outstanding_CSV_FileName</t>
-  </si>
-  <si>
-    <t>CCB_LIQ_SYD_VLS_CUSTOMER_20190419</t>
   </si>
   <si>
     <t>CCB_LIQ_SYD_VLS_OUTSTANDING_20190419</t>
@@ -464,6 +461,33 @@
   </si>
   <si>
     <t>DataSet\Integration_DataSet\Extracts\DWE_LIQ\Decrypted_Files\Zone3</t>
+  </si>
+  <si>
+    <t>Test_Case</t>
+  </si>
+  <si>
+    <t>DWELIQ_FuncVal02_Z2</t>
+  </si>
+  <si>
+    <t>DWELIQ_FuncVal02_Z3</t>
+  </si>
+  <si>
+    <t>CCB_LIQ_SYD_VLS_CUSTOMER_</t>
+  </si>
+  <si>
+    <t>CCB_LIQ_SYD_VLS_OUTSTANDING_</t>
+  </si>
+  <si>
+    <t>C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DWE_LIQ\DWE_LIQ_Extracts\DWELIQ_Multi_E2E_001\ZONE2\</t>
+  </si>
+  <si>
+    <t>C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DWE_LIQ\DWE_LIQ_Extracts\DWELIQ_Multi_E2E_001\ZONE3\</t>
+  </si>
+  <si>
+    <t>CCB_LIQ_EUR_VLS_CUSTOMER_</t>
+  </si>
+  <si>
+    <t>CCB_LIQ_EUR_VLS_OUTSTANDING_</t>
   </si>
 </sst>
 </file>
@@ -866,8 +890,8 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,51 +936,51 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -993,7 +1017,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1001,18 +1025,18 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1049,13 +1073,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1063,16 +1087,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1109,13 +1133,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1123,16 +1147,16 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1168,7 +1192,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1176,18 +1200,18 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1225,13 +1249,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1239,24 +1263,24 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1293,10 +1317,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1304,21 +1328,21 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1386,103 +1410,103 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>80</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
@@ -1490,114 +1514,114 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AF2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1635,13 +1659,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="195" customHeight="1" x14ac:dyDescent="0.25">
@@ -1649,24 +1673,24 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1702,7 +1726,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1710,18 +1734,18 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1761,7 +1785,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1776,57 +1800,74 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="115.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>138</v>
+      <c r="B2" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -1857,13 +1898,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1877,7 +1918,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1911,13 +1952,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1931,7 +1972,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1968,13 +2009,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1982,24 +2023,24 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>126</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2041,7 +2082,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
@@ -2052,10 +2093,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2"/>
       <c r="K2" s="5"/>
@@ -2064,10 +2105,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2109,7 +2150,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
@@ -2120,10 +2161,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2"/>
       <c r="K2" s="5"/>
@@ -2132,10 +2173,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2177,7 +2218,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
@@ -2188,10 +2229,10 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" s="2"/>
       <c r="K2" s="5"/>
@@ -2200,10 +2241,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2238,7 +2279,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2246,18 +2287,18 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2293,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2301,7 +2342,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -2309,10 +2350,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2350,7 +2391,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2360,20 +2401,20 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2411,13 +2452,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="128.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,24 +2466,24 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GDE-6677 data set update
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DWE_LIQ/DWELIQ_Functional_TestData.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DWE_LIQ/DWELIQ_Functional_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="29670" yWindow="4455" windowWidth="28320" windowHeight="8295" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FuncVal01" sheetId="1" state="visible" r:id="rId1"/>
@@ -2052,13 +2052,13 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="21.42578125" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="116.7109375" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="128.7109375" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
     <col width="23.7109375" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
     <col width="15.5703125" customWidth="1" style="5" min="5" max="5"/>
     <col width="19.5703125" customWidth="1" style="5" min="6" max="6"/>
@@ -2111,7 +2111,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DWE_LIQ\DWE_LIQ_Extracts\DWELIQ_Multi_E2E_001\ZONE2\</t>
+          <t>C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DWE_LIQ\DWE_LIQ_Extracts\DWELIQ_Multi_E2E_001\ZONE2\CCB_LIQ_EUR_</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DWE_LIQ\DWE_LIQ_Extracts\DWELIQ_Multi_E2E_001\ZONE3\</t>
+          <t>C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DWE_LIQ\DWE_LIQ_Extracts\DWELIQ_Multi_E2E_001\ZONE3\CCB_LIQ_SYD_</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">

</xml_diff>

<commit_message>
GDE-6676 Code and DataSet Updates
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/Extracts/DWE_LIQ/DWELIQ_Functional_TestData.xlsx
+++ b/DataSet/Integration_DataSet/Extracts/DWE_LIQ/DWELIQ_Functional_TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FuncVal01" sheetId="1" state="visible" r:id="rId1"/>
@@ -425,22 +425,23 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="6.140625" customWidth="1" style="2" min="1" max="1"/>
-    <col width="66.28515625" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
-    <col width="42.140625" customWidth="1" style="2" min="3" max="3"/>
-    <col width="40.7109375" customWidth="1" style="2" min="4" max="4"/>
-    <col width="43.28515625" customWidth="1" style="2" min="5" max="5"/>
-    <col width="35" customWidth="1" style="2" min="6" max="7"/>
-    <col width="37.5703125" customWidth="1" style="2" min="8" max="8"/>
-    <col width="14" bestFit="1" customWidth="1" min="9" max="9"/>
+    <col width="21.42578125" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="129.85546875" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="42.140625" customWidth="1" style="2" min="4" max="4"/>
+    <col width="40.7109375" customWidth="1" style="2" min="5" max="5"/>
+    <col width="43.28515625" customWidth="1" style="2" min="6" max="6"/>
+    <col width="35" customWidth="1" style="2" min="7" max="8"/>
+    <col width="37.5703125" customWidth="1" style="2" min="9" max="9"/>
+    <col width="14" bestFit="1" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="2">
@@ -451,40 +452,45 @@
       </c>
       <c r="B1" s="4" t="inlineStr">
         <is>
+          <t>Test_Case</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
           <t>CSV_FilePath</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Bal_Subledger_CSV_FileName</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>GL_Account_Num_CSV_FileName</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>GL_Short_Name_CSV_FileName</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>Branch_CSV_FileName</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>Expense_CSV_FileName</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>Portfolio_CSV_FileName</t>
         </is>
       </c>
-      <c r="I1" s="10" t="inlineStr">
+      <c r="J1" s="10" t="inlineStr">
         <is>
           <t>Business_Date</t>
         </is>
@@ -496,39 +502,49 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>DataSet\Integration_DataSet\Extracts\DWE_LIQ\Decrypted_Files\Zone2</t>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>DWELIQ_FuncVal01_Z3</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_BAL_SUBLEDGER_20200320</t>
+          <t>C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DWE_LIQ\DWE_LIQ_Extracts\DWELIQ_Multi_E2E_001\ZONE3\CCB_LIQ_SYD_</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_GL_ACCT_NUM_20200320</t>
+          <t>CCB_LIQ_SYD_VLS_BAL_SUBLEDGER_</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_GL_SHORT_NAME_20200320</t>
+          <t>CCB_LIQ_SYD_VLS_GL_ACCT_NUM_</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_BRANCH_20200320</t>
+          <t>CCB_LIQ_SYD_VLS_GL_SHORT_NAME_</t>
         </is>
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_EXPENSE_20200320</t>
+          <t>CCB_LIQ_SYD_VLS_BRANCH_</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_PORTFOLIO_20200320</t>
+          <t>CCB_LIQ_SYD_VLS_EXPENSE_</t>
+        </is>
+      </c>
+      <c r="I2" s="2" t="inlineStr">
+        <is>
+          <t>CCB_LIQ_SYD_VLS_PORTFOLIO_</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>20210120</t>
         </is>
       </c>
     </row>
@@ -538,39 +554,49 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>DataSet\Integration_DataSet\Extracts\DWE_LIQ\Decrypted_Files\Zone3</t>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>DWELIQ_FuncVal01_Z2</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_BAL_SUBLEDGER_20200320</t>
+          <t>C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\Extracts\DWE_LIQ\DWE_LIQ_Extracts\DWELIQ_Multi_E2E_002\ZONE2\CCB_LIQ_EUR_</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_GL_ACCT_NUM_20200320</t>
+          <t>CCB_LIQ_EUR_VLS_BAL_SUBLEDGER_</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_GL_SHORT_NAME_20200320</t>
+          <t>CCB_LIQ_EUR_VLS_GL_ACCT_NUM_</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_BRANCH_20200320</t>
+          <t>CCB_LIQ_EUR_VLS_GL_SHORT_NAME_</t>
         </is>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_EXPENSE_20200320</t>
+          <t>CCB_LIQ_EUR_VLS_BRANCH_</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
-          <t>CCB_LIQ_SYD_VLS_PORTFOLIO_20200320</t>
+          <t>CCB_LIQ_EUR_VLS_EXPENSE_</t>
+        </is>
+      </c>
+      <c r="I3" s="2" t="inlineStr">
+        <is>
+          <t>CCB_LIQ_EUR_VLS_PORTFOLIO_</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>20200709</t>
         </is>
       </c>
     </row>
@@ -1713,8 +1739,8 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>